<commit_message>
fixed time bug in the input file
</commit_message>
<xml_diff>
--- a/mesta_input.xlsx
+++ b/mesta_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\_1\python\cestaky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{693A92AD-50B6-43B6-A2D2-968DAAFCF4FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771591CF-A9C4-49AA-B729-D848879F0780}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,11 +506,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -844,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:LH2556"/>
+  <dimension ref="A1:LH2557"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A2502" sqref="A2502:D2556"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1371,7 +1372,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="AX11" s="1"/>
     </row>
@@ -37056,6 +37057,11 @@
       </c>
       <c r="D2556" s="1">
         <v>1.388888888888889E-2</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2557" s="4">
+        <v>0.95743055555555545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>